<commit_message>
Correzione checklist RSA, RIS, LIS
Correzione checklist RSA, RIS, LIS
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111CHORUSSRLXX/CHORUS_SRL/ACCDIALAB_LIS/V2023/report-checklist.xlsx
+++ b/GATEWAY/A1#111CHORUSSRLXX/CHORUS_SRL/ACCDIALAB_LIS/V2023/report-checklist.xlsx
@@ -460,9 +460,6 @@
     <t>16:58</t>
   </si>
   <si>
-    <t>In caso di timeout con il gateway il processo clinico continua e il referto viene prodotto. Quest'ultimo viene aggiunto in una coda dalla quale l’operatore può effettuare nuovamente l’invio una volta che il gateway torna disponibile.</t>
-  </si>
-  <si>
     <t>Il caso non è applicabile, il campo da testare è obbligatorio nell'applicativo che genera il CDA2</t>
   </si>
   <si>
@@ -551,6 +548,9 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.150.4.4.f799db888f705c432f32622d943a9ffb8f0cf65fc5a1fde26d056ac2700e4997.fcce16f038^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>In caso di timeout con il gateway il processo clinico continua e il referto viene prodotto. Quest'ultimo viene aggiunto in una coda dalla quale il medico può effettuare nuovamente l’invio una volta che il gateway torna disponibile.</t>
   </si>
 </sst>
 </file>
@@ -1449,7 +1449,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T604"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="J10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1467,7 +1469,7 @@
     <col min="12" max="12" width="14.28515625" style="58" customWidth="1"/>
     <col min="13" max="13" width="10.7109375" style="58" customWidth="1"/>
     <col min="14" max="14" width="114.85546875" style="58" customWidth="1"/>
-    <col min="15" max="15" width="8.5703125" style="58" customWidth="1"/>
+    <col min="15" max="15" width="32.7109375" style="58" customWidth="1"/>
     <col min="16" max="16" width="114.140625" style="58" customWidth="1"/>
     <col min="17" max="17" width="7.85546875" style="58" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="13.28515625" style="58" customWidth="1"/>
@@ -1746,13 +1748,13 @@
         <v>45237</v>
       </c>
       <c r="G10" s="39" t="s">
+        <v>119</v>
+      </c>
+      <c r="H10" s="40" t="s">
         <v>120</v>
       </c>
-      <c r="H10" s="40" t="s">
+      <c r="I10" s="40" t="s">
         <v>121</v>
-      </c>
-      <c r="I10" s="40" t="s">
-        <v>122</v>
       </c>
       <c r="J10" s="41" t="s">
         <v>26</v>
@@ -1790,13 +1792,13 @@
         <v>45237</v>
       </c>
       <c r="G11" s="45" t="s">
+        <v>122</v>
+      </c>
+      <c r="H11" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="H11" s="46" t="s">
+      <c r="I11" s="46" t="s">
         <v>124</v>
-      </c>
-      <c r="I11" s="46" t="s">
-        <v>125</v>
       </c>
       <c r="J11" s="41" t="s">
         <v>26</v>
@@ -1834,13 +1836,13 @@
         <v>45237</v>
       </c>
       <c r="G12" s="45" t="s">
+        <v>125</v>
+      </c>
+      <c r="H12" s="46" t="s">
         <v>126</v>
       </c>
-      <c r="H12" s="46" t="s">
+      <c r="I12" s="46" t="s">
         <v>127</v>
-      </c>
-      <c r="I12" s="46" t="s">
-        <v>128</v>
       </c>
       <c r="J12" s="41" t="s">
         <v>26</v>
@@ -1878,13 +1880,13 @@
         <v>45237</v>
       </c>
       <c r="G13" s="45" t="s">
+        <v>128</v>
+      </c>
+      <c r="H13" s="46" t="s">
         <v>129</v>
       </c>
-      <c r="H13" s="46" t="s">
+      <c r="I13" s="46" t="s">
         <v>130</v>
-      </c>
-      <c r="I13" s="46" t="s">
-        <v>131</v>
       </c>
       <c r="J13" s="41" t="s">
         <v>26</v>
@@ -1922,13 +1924,13 @@
         <v>45237</v>
       </c>
       <c r="G14" s="50" t="s">
+        <v>131</v>
+      </c>
+      <c r="H14" s="68" t="s">
         <v>132</v>
       </c>
-      <c r="H14" s="68" t="s">
+      <c r="I14" s="51" t="s">
         <v>133</v>
-      </c>
-      <c r="I14" s="51" t="s">
-        <v>134</v>
       </c>
       <c r="J14" s="51" t="s">
         <v>26</v>
@@ -2069,7 +2071,7 @@
       <c r="N17" s="41"/>
       <c r="O17" s="41"/>
       <c r="P17" s="55" t="s">
-        <v>104</v>
+        <v>134</v>
       </c>
       <c r="Q17" s="41"/>
       <c r="R17" s="42" t="s">
@@ -2104,7 +2106,7 @@
         <v>37</v>
       </c>
       <c r="K18" s="55" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L18" s="41"/>
       <c r="M18" s="41"/>
@@ -2142,7 +2144,7 @@
         <v>37</v>
       </c>
       <c r="K19" s="55" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L19" s="41"/>
       <c r="M19" s="41"/>
@@ -2176,13 +2178,13 @@
         <v>45230</v>
       </c>
       <c r="G20" s="45" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H20" s="46" t="s">
+        <v>106</v>
+      </c>
+      <c r="I20" s="46" t="s">
         <v>107</v>
-      </c>
-      <c r="I20" s="46" t="s">
-        <v>108</v>
       </c>
       <c r="J20" s="41" t="s">
         <v>26</v>
@@ -2198,7 +2200,7 @@
         <v>50</v>
       </c>
       <c r="O20" s="41" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="P20" s="55" t="s">
         <v>51</v>
@@ -2229,13 +2231,13 @@
         <v>45230</v>
       </c>
       <c r="G21" s="45" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H21" s="46" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I21" s="46" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J21" s="41" t="s">
         <v>26</v>
@@ -2287,7 +2289,7 @@
         <v>37</v>
       </c>
       <c r="K22" s="55" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L22" s="41"/>
       <c r="M22" s="41"/>
@@ -2325,7 +2327,7 @@
         <v>37</v>
       </c>
       <c r="K23" s="55" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L23" s="41"/>
       <c r="M23" s="41"/>
@@ -2363,7 +2365,7 @@
         <v>37</v>
       </c>
       <c r="K24" s="55" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L24" s="41"/>
       <c r="M24" s="41"/>
@@ -2401,7 +2403,7 @@
         <v>37</v>
       </c>
       <c r="K25" s="55" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L25" s="41"/>
       <c r="M25" s="41"/>
@@ -2439,7 +2441,7 @@
         <v>37</v>
       </c>
       <c r="K26" s="55" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L26" s="41"/>
       <c r="M26" s="41"/>
@@ -2473,13 +2475,13 @@
         <v>45231</v>
       </c>
       <c r="G27" s="45" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H27" s="46" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I27" s="46" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J27" s="41" t="s">
         <v>26</v>
@@ -2530,10 +2532,10 @@
         <v>103</v>
       </c>
       <c r="H28" s="46" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I28" s="46" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J28" s="41" t="s">
         <v>26</v>
@@ -15248,7 +15250,7 @@
       <formula1>"SI,NO"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J10:J21 L10:M28 O10:O20 O22:O26 J27:J28 Q10:Q19 Q21:Q28">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J10:J21 L10:M28 Q21:Q28 O22:O26 J27:J28 Q10:Q19 O10:O20">
       <formula1>#REF!</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>